<commit_message>
Resultados experimentos prob verif
</commit_message>
<xml_diff>
--- a/Codes/Tesis/LocalSearch/ExperimentosProbVerif.xlsx
+++ b/Codes/Tesis/LocalSearch/ExperimentosProbVerif.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\EstudiosProfesionales\FIME\Doctorado\TesisDoctoral\Codes\Tesis\LocalSearch\Exp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\EstudiosProfesionales\FIME\Doctorado\TesisDoctoral\Codes\Tesis\LocalSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02793BF8-BFB1-435F-AFCF-300E2E0B939A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489D6A02-F121-4E2A-A517-B3906575623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F9B03A0-B3B8-4176-BEA4-1A200B2F55D7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -108,13 +108,16 @@
   </si>
   <si>
     <t>prob verif</t>
+  </si>
+  <si>
+    <t>Instance_500_50_200_6_6_Exp1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +135,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,9 +162,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9534132-7682-4764-98D8-4CB2B3319028}">
-  <dimension ref="B2:G19"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,348 +518,368 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.23400000000003918</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1474.6523947715759</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3644.1554698944092</v>
-      </c>
-      <c r="F3" s="1">
-        <v>100</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2.01E-2</v>
+        <v>23</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.2905500000002039</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2998.6013467311859</v>
+      </c>
+      <c r="E3" s="2">
+        <v>36062.218600749969</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.3163500000000391</v>
+        <v>1.9176500000002452</v>
       </c>
       <c r="D4" s="1">
-        <v>6.6082239151000977</v>
+        <v>2930.4411442279816</v>
       </c>
       <c r="E4" s="1">
-        <v>583.41085076332092</v>
+        <v>36292.000036716461</v>
       </c>
       <c r="F4" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>0.3163500000000391</v>
+        <v>1.6748500000003281</v>
       </c>
       <c r="D5" s="1">
-        <v>49.67138934135437</v>
+        <v>2621.4234056472778</v>
       </c>
       <c r="E5" s="1">
-        <v>824.30037069320679</v>
+        <v>37491.125707149506</v>
       </c>
       <c r="F5" s="1">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>0.3163500000000391</v>
+        <v>1.4720500000001464</v>
       </c>
       <c r="D6" s="1">
-        <v>101.45193409919739</v>
+        <v>4094.0508749485016</v>
       </c>
       <c r="E6" s="1">
-        <v>575.3419942855835</v>
+        <v>36107.437313079834</v>
       </c>
       <c r="F6" s="1">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>0.3163500000000391</v>
+        <v>0.46315000000003914</v>
       </c>
       <c r="D7" s="1">
-        <v>199.17367959022522</v>
+        <v>137.61068916320801</v>
       </c>
       <c r="E7" s="1">
-        <v>562.06618976593018</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>0.05</v>
+        <v>581.0126850605011</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.04</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>0.3163500000000391</v>
+        <v>0.46315000000003914</v>
       </c>
       <c r="D8" s="1">
-        <v>230.96132373809814</v>
+        <v>1853.6293318271637</v>
       </c>
       <c r="E8" s="1">
-        <v>575.10294246673584</v>
+        <v>4372.7078351974487</v>
       </c>
       <c r="F8" s="1">
         <v>100</v>
       </c>
       <c r="G8" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>0.3163500000000391</v>
+        <v>0.46315000000003914</v>
       </c>
       <c r="D9" s="1">
-        <v>256.00622940063477</v>
+        <v>87.200529098510742</v>
       </c>
       <c r="E9" s="1">
-        <v>594.77859950065613</v>
+        <v>3208.2129061222076</v>
       </c>
       <c r="F9" s="1">
         <v>100</v>
       </c>
       <c r="G9" s="1">
-        <v>2.3E-2</v>
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>0.3163500000000391</v>
+        <v>0.46315000000003914</v>
       </c>
       <c r="D10" s="1">
-        <v>284.06933999061584</v>
+        <v>940.52506399154663</v>
       </c>
       <c r="E10" s="1">
-        <v>820.08562397956848</v>
+        <v>2361.3871066570282</v>
       </c>
       <c r="F10" s="1">
         <v>100</v>
       </c>
       <c r="G10" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>0.3163500000000391</v>
+        <v>0.37785000000003921</v>
       </c>
       <c r="D11" s="1">
-        <v>571.76856184005737</v>
+        <v>1506.6729125976563</v>
       </c>
       <c r="E11" s="1">
-        <v>1854.7529611587524</v>
+        <v>4889.0646033287048</v>
       </c>
       <c r="F11" s="1">
         <v>100</v>
       </c>
       <c r="G11" s="1">
-        <v>2.0500000000000001E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>0.37785000000003921</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D12" s="1">
-        <v>1506.6729125976563</v>
+        <v>230.96132373809814</v>
       </c>
       <c r="E12" s="1">
-        <v>4889.0646033287048</v>
+        <v>575.10294246673584</v>
       </c>
       <c r="F12" s="1">
         <v>100</v>
       </c>
       <c r="G12" s="1">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>0.46315000000003914</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D13" s="1">
-        <v>87.200529098510742</v>
+        <v>6.6082239151000977</v>
       </c>
       <c r="E13" s="1">
-        <v>3208.2129061222076</v>
+        <v>583.41085076332092</v>
       </c>
       <c r="F13" s="1">
         <v>100</v>
       </c>
       <c r="G13" s="1">
-        <v>2.0199999999999999E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>0.46315000000003914</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D14" s="1">
-        <v>137.61068916320801</v>
+        <v>199.17367959022522</v>
       </c>
       <c r="E14" s="1">
-        <v>581.0126850605011</v>
-      </c>
-      <c r="F14" s="1">
-        <v>100</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.04</v>
+        <v>562.06618976593018</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
-        <v>0.46315000000003914</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D15" s="1">
-        <v>940.52506399154663</v>
+        <v>49.67138934135437</v>
       </c>
       <c r="E15" s="1">
-        <v>2361.3871066570282</v>
+        <v>824.30037069320679</v>
       </c>
       <c r="F15" s="1">
         <v>100</v>
       </c>
       <c r="G15" s="1">
-        <v>2.0299999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>0.46315000000003914</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D16" s="1">
-        <v>1853.6293318271637</v>
+        <v>571.76856184005737</v>
       </c>
       <c r="E16" s="1">
-        <v>4372.7078351974487</v>
+        <v>1854.7529611587524</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
       </c>
       <c r="G16" s="1">
-        <v>0.02</v>
+        <v>2.0500000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>1.4720500000001464</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D17" s="1">
-        <v>4094.0508749485016</v>
+        <v>284.06933999061584</v>
       </c>
       <c r="E17" s="1">
-        <v>36107.437313079834</v>
+        <v>820.08562397956848</v>
       </c>
       <c r="F17" s="1">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G17" s="1">
-        <v>0.01</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1">
-        <v>1.6748500000003281</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D18" s="1">
-        <v>2621.4234056472778</v>
+        <v>101.45193409919739</v>
       </c>
       <c r="E18" s="1">
-        <v>37491.125707149506</v>
+        <v>575.3419942855835</v>
       </c>
       <c r="F18" s="1">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="G18" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1">
-        <v>1.9176500000002452</v>
+        <v>0.3163500000000391</v>
       </c>
       <c r="D19" s="1">
-        <v>2930.4411442279816</v>
+        <v>256.00622940063477</v>
       </c>
       <c r="E19" s="1">
-        <v>36292.000036716461</v>
+        <v>594.77859950065613</v>
       </c>
       <c r="F19" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G19" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.23400000000003918</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1474.6523947715759</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3644.1554698944092</v>
+      </c>
+      <c r="F20" s="1">
+        <v>100</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2.01E-2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:G2" xr:uid="{B9534132-7682-4764-98D8-4CB2B3319028}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G19">
-      <sortCondition ref="C2"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G20">
+      <sortCondition descending="1" ref="C2"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>